<commit_message>
Campos nuevos de geolocalización
</commit_message>
<xml_diff>
--- a/AVON APP - MEDICIONES DE TRAFICO.xlsx
+++ b/AVON APP - MEDICIONES DE TRAFICO.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Flutter\avon_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3436D8CF-5C4B-4118-8E20-43CB2CAC5CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EE8C43-5537-4EC0-B5B8-9722E12A8AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{501DC589-9CD0-4CFF-B6D2-558773053F13}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{501DC589-9CD0-4CFF-B6D2-558773053F13}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -301,6 +302,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A9E8AA2-8593-4AA0-B407-1A58F86614E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5341620" cy="3627120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -602,7 +669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D08E91B-D980-48D4-9238-DEB673C3562A}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1038,4 +1105,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{009F6367-8227-400F-A478-9E95E6BBE420}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>